<commit_message>
update - packs/unit to packs/case label
</commit_message>
<xml_diff>
--- a/core/seed_companies_company.xlsx
+++ b/core/seed_companies_company.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.cheng\Documents\Visual Studio Code\Django\tsmb_sys01_repo01\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE40D92-F421-488E-8767-422CDC0A5228}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC9C81C-A144-4E3F-8D67-8A04E12B7427}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,10 @@
     <t>NAME</t>
   </si>
   <si>
-    <t>SM</t>
+    <t>PHC</t>
   </si>
   <si>
-    <t>VG</t>
+    <t>VFI</t>
   </si>
 </sst>
 </file>

</xml_diff>